<commit_message>
Final Commit for Dividing the each output to new row
</commit_message>
<xml_diff>
--- a/input/test.xlsx
+++ b/input/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -277,14 +277,11 @@
   </sheetPr>
   <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z5" activeCellId="0" sqref="Z5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE2" activeCellId="0" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -456,9 +453,6 @@
       </c>
       <c r="AD2" s="0" t="s">
         <v>2</v>
-      </c>
-      <c r="AE2" s="0" t="n">
-        <v>700</v>
       </c>
       <c r="AF2" s="0" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
added threshold-used in output
</commit_message>
<xml_diff>
--- a/input/test.xlsx
+++ b/input/test.xlsx
@@ -277,11 +277,14 @@
   </sheetPr>
   <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AE2" activeCellId="0" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -453,6 +456,9 @@
       </c>
       <c r="AD2" s="0" t="s">
         <v>2</v>
+      </c>
+      <c r="AE2" s="0" t="n">
+        <v>2000</v>
       </c>
       <c r="AF2" s="0" t="s">
         <v>39</v>

</xml_diff>